<commit_message>
v0.3.0; new images, functionalities page, and more
</commit_message>
<xml_diff>
--- a/public/StructureDefinition-Environmental.xlsx
+++ b/public/StructureDefinition-Environmental.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.1</t>
+    <t>0.3.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-27T18:16:54-05:00</t>
+    <t>2022-03-28T04:09:55-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>